<commit_message>
ng: update epi forms
</commit_message>
<xml_diff>
--- a/ONCHO/Entomological survey Survey/Nigeria/2023/june/ng_oncho_stop_4_site_202306.xlsx
+++ b/ONCHO/Entomological survey Survey/Nigeria/2023/june/ng_oncho_stop_4_site_202306.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\ONCHO\Entomological survey Survey\Nigeria\2023\june\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413D4195-F50F-442B-B812-2A85D7C05703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0644F793-3160-4B62-B997-C48996B49FFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="164">
   <si>
     <t>type</t>
   </si>
@@ -372,12 +372,6 @@
     <t>English</t>
   </si>
   <si>
-    <t>ng_oncho_stop_4_site_202306</t>
-  </si>
-  <si>
-    <t>(2023 June) - 4. Site Form</t>
-  </si>
-  <si>
     <t>CROSS RIVER</t>
   </si>
   <si>
@@ -462,12 +456,6 @@
     <t>ABARAGBA</t>
   </si>
   <si>
-    <t>BASSINGE</t>
-  </si>
-  <si>
-    <t>BAYALUGA</t>
-  </si>
-  <si>
     <t>BUANCHOR</t>
   </si>
   <si>
@@ -480,13 +468,52 @@
     <t>EDONDON</t>
   </si>
   <si>
-    <t>BEBI</t>
-  </si>
-  <si>
     <t>AGOI IBAMI</t>
   </si>
   <si>
-    <t>OTUKPO</t>
+    <t>(2023 June) - 4. Site Form V2</t>
+  </si>
+  <si>
+    <t>ng_oncho_stop_4_site_202306_v2</t>
+  </si>
+  <si>
+    <t>ODUKPANI</t>
+  </si>
+  <si>
+    <t>ANINGEJE</t>
+  </si>
+  <si>
+    <t>IKOT OKPORA</t>
+  </si>
+  <si>
+    <t>ABIJANG</t>
+  </si>
+  <si>
+    <t>BASSENGE</t>
+  </si>
+  <si>
+    <t>BAYULUGA</t>
+  </si>
+  <si>
+    <t>BEBI (BEMIAH)</t>
+  </si>
+  <si>
+    <t>BIKAA</t>
+  </si>
+  <si>
+    <t>BIMAH</t>
+  </si>
+  <si>
+    <t>BETUKWEL</t>
+  </si>
+  <si>
+    <t>ATAN-OKONYONG</t>
+  </si>
+  <si>
+    <t>EZELENG (SHINGILE)</t>
+  </si>
+  <si>
+    <t>UTUKPO</t>
   </si>
 </sst>
 </file>
@@ -513,7 +540,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1404,11 +1431,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F86"/>
+  <dimension ref="A1:F103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A63" sqref="A63:A86"/>
+      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A95" sqref="A95:A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1701,10 +1728,10 @@
         <v>87</v>
       </c>
       <c r="B23" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C23" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1712,13 +1739,13 @@
         <v>88</v>
       </c>
       <c r="B25" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C25" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1726,13 +1753,13 @@
         <v>88</v>
       </c>
       <c r="B26" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C26" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1740,13 +1767,13 @@
         <v>88</v>
       </c>
       <c r="B27" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C27" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1754,13 +1781,13 @@
         <v>88</v>
       </c>
       <c r="B28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1768,13 +1795,13 @@
         <v>88</v>
       </c>
       <c r="B29" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C29" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1782,13 +1809,13 @@
         <v>88</v>
       </c>
       <c r="B30" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C30" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1796,13 +1823,13 @@
         <v>88</v>
       </c>
       <c r="B31" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C31" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1810,13 +1837,13 @@
         <v>88</v>
       </c>
       <c r="B32" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C32" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1824,13 +1851,13 @@
         <v>88</v>
       </c>
       <c r="B33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1838,13 +1865,13 @@
         <v>88</v>
       </c>
       <c r="B34" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C34" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1852,13 +1879,13 @@
         <v>88</v>
       </c>
       <c r="B35" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
       <c r="C35" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
       <c r="D35" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1866,27 +1893,27 @@
         <v>88</v>
       </c>
       <c r="B36" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C36" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D36" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" t="s">
-        <v>89</v>
-      </c>
-      <c r="B38" t="s">
-        <v>131</v>
-      </c>
-      <c r="C38" t="s">
-        <v>131</v>
-      </c>
-      <c r="E38" t="s">
-        <v>119</v>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>88</v>
+      </c>
+      <c r="B37" t="s">
+        <v>128</v>
+      </c>
+      <c r="C37" t="s">
+        <v>128</v>
+      </c>
+      <c r="D37" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1894,13 +1921,13 @@
         <v>89</v>
       </c>
       <c r="B39" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C39" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E39" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1908,13 +1935,13 @@
         <v>89</v>
       </c>
       <c r="B40" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C40" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E40" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1922,13 +1949,13 @@
         <v>89</v>
       </c>
       <c r="B41" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="C41" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="E41" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1936,13 +1963,13 @@
         <v>89</v>
       </c>
       <c r="B42" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C42" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E42" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1950,13 +1977,13 @@
         <v>89</v>
       </c>
       <c r="B43" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C43" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E43" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1964,13 +1991,13 @@
         <v>89</v>
       </c>
       <c r="B44" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C44" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E44" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1978,13 +2005,13 @@
         <v>89</v>
       </c>
       <c r="B45" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C45" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E45" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1992,13 +2019,13 @@
         <v>89</v>
       </c>
       <c r="B46" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C46" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E46" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -2006,13 +2033,13 @@
         <v>89</v>
       </c>
       <c r="B47" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C47" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E47" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -2020,321 +2047,321 @@
         <v>89</v>
       </c>
       <c r="B48" t="s">
+        <v>153</v>
+      </c>
+      <c r="C48" t="s">
+        <v>153</v>
+      </c>
+      <c r="E48" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>89</v>
+      </c>
+      <c r="B49" t="s">
+        <v>137</v>
+      </c>
+      <c r="C49" t="s">
+        <v>137</v>
+      </c>
+      <c r="E49" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>89</v>
+      </c>
+      <c r="B50" t="s">
+        <v>144</v>
+      </c>
+      <c r="C50" t="s">
+        <v>144</v>
+      </c>
+      <c r="E50" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>89</v>
+      </c>
+      <c r="B51" t="s">
+        <v>138</v>
+      </c>
+      <c r="C51" t="s">
+        <v>138</v>
+      </c>
+      <c r="E51" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>89</v>
+      </c>
+      <c r="B52" t="s">
+        <v>139</v>
+      </c>
+      <c r="C52" t="s">
+        <v>139</v>
+      </c>
+      <c r="E52" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>89</v>
+      </c>
+      <c r="B53" t="s">
+        <v>140</v>
+      </c>
+      <c r="C53" t="s">
+        <v>140</v>
+      </c>
+      <c r="E53" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>89</v>
+      </c>
+      <c r="B54" t="s">
+        <v>154</v>
+      </c>
+      <c r="C54" t="s">
+        <v>154</v>
+      </c>
+      <c r="E54" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>89</v>
+      </c>
+      <c r="B55" t="s">
         <v>141</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C55" t="s">
         <v>141</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E55" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>89</v>
+      </c>
+      <c r="B56" t="s">
+        <v>142</v>
+      </c>
+      <c r="C56" t="s">
+        <v>142</v>
+      </c>
+      <c r="E56" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>89</v>
+      </c>
+      <c r="B57" t="s">
+        <v>143</v>
+      </c>
+      <c r="C57" t="s">
+        <v>143</v>
+      </c>
+      <c r="E57" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
-      <c r="A49" t="s">
-        <v>89</v>
-      </c>
-      <c r="B49" t="s">
-        <v>142</v>
-      </c>
-      <c r="C49" t="s">
-        <v>142</v>
-      </c>
-      <c r="E49" t="s">
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>89</v>
+      </c>
+      <c r="B58" t="s">
+        <v>155</v>
+      </c>
+      <c r="C58" t="s">
+        <v>155</v>
+      </c>
+      <c r="E58" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
-      <c r="A50" t="s">
-        <v>89</v>
-      </c>
-      <c r="B50" t="s">
-        <v>143</v>
-      </c>
-      <c r="C50" t="s">
-        <v>143</v>
-      </c>
-      <c r="E50" t="s">
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>89</v>
+      </c>
+      <c r="B59" t="s">
+        <v>156</v>
+      </c>
+      <c r="C59" t="s">
+        <v>156</v>
+      </c>
+      <c r="E59" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
-      <c r="A51" t="s">
-        <v>89</v>
-      </c>
-      <c r="B51" t="s">
-        <v>144</v>
-      </c>
-      <c r="C51" t="s">
-        <v>144</v>
-      </c>
-      <c r="E51" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" t="s">
-        <v>89</v>
-      </c>
-      <c r="B52" t="s">
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>89</v>
+      </c>
+      <c r="B60" t="s">
+        <v>157</v>
+      </c>
+      <c r="C60" t="s">
+        <v>157</v>
+      </c>
+      <c r="E60" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>89</v>
+      </c>
+      <c r="B61" t="s">
+        <v>158</v>
+      </c>
+      <c r="C61" t="s">
+        <v>158</v>
+      </c>
+      <c r="E61" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>89</v>
+      </c>
+      <c r="B62" t="s">
+        <v>159</v>
+      </c>
+      <c r="C62" t="s">
+        <v>159</v>
+      </c>
+      <c r="E62" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>89</v>
+      </c>
+      <c r="B63" t="s">
         <v>145</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C63" t="s">
         <v>145</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E63" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
-      <c r="A53" t="s">
-        <v>89</v>
-      </c>
-      <c r="B53" t="s">
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>89</v>
+      </c>
+      <c r="B64" t="s">
         <v>146</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C64" t="s">
         <v>146</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E64" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" t="s">
+        <v>89</v>
+      </c>
+      <c r="B65" t="s">
+        <v>147</v>
+      </c>
+      <c r="C65" t="s">
+        <v>147</v>
+      </c>
+      <c r="E65" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
-      <c r="A54" t="s">
-        <v>89</v>
-      </c>
-      <c r="B54" t="s">
-        <v>147</v>
-      </c>
-      <c r="C54" t="s">
-        <v>147</v>
-      </c>
-      <c r="E54" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" t="s">
-        <v>89</v>
-      </c>
-      <c r="B55" t="s">
+    <row r="66" spans="1:6">
+      <c r="A66" t="s">
+        <v>89</v>
+      </c>
+      <c r="B66" t="s">
+        <v>160</v>
+      </c>
+      <c r="C66" t="s">
+        <v>160</v>
+      </c>
+      <c r="E66" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" t="s">
+        <v>89</v>
+      </c>
+      <c r="B67" t="s">
+        <v>161</v>
+      </c>
+      <c r="C67" t="s">
+        <v>161</v>
+      </c>
+      <c r="E67" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" t="s">
+        <v>89</v>
+      </c>
+      <c r="B68" t="s">
         <v>148</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C68" t="s">
         <v>148</v>
       </c>
-      <c r="E55" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" t="s">
-        <v>89</v>
-      </c>
-      <c r="B56" t="s">
-        <v>149</v>
-      </c>
-      <c r="C56" t="s">
-        <v>149</v>
-      </c>
-      <c r="E56" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57" t="s">
-        <v>89</v>
-      </c>
-      <c r="B57" t="s">
-        <v>150</v>
-      </c>
-      <c r="C57" t="s">
-        <v>150</v>
-      </c>
-      <c r="E57" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58" t="s">
-        <v>89</v>
-      </c>
-      <c r="B58" t="s">
-        <v>151</v>
-      </c>
-      <c r="C58" t="s">
-        <v>151</v>
-      </c>
-      <c r="E58" t="s">
+      <c r="E68" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
-      <c r="A59" t="s">
-        <v>89</v>
-      </c>
-      <c r="B59" t="s">
-        <v>152</v>
-      </c>
-      <c r="C59" t="s">
-        <v>152</v>
-      </c>
-      <c r="E59" t="s">
+    <row r="69" spans="1:6">
+      <c r="A69" t="s">
+        <v>89</v>
+      </c>
+      <c r="B69" t="s">
+        <v>162</v>
+      </c>
+      <c r="C69" t="s">
+        <v>162</v>
+      </c>
+      <c r="E69" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
-      <c r="A60" t="s">
-        <v>89</v>
-      </c>
-      <c r="B60" t="s">
-        <v>153</v>
-      </c>
-      <c r="C60" t="s">
-        <v>153</v>
-      </c>
-      <c r="E60" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
-      <c r="A61" t="s">
-        <v>89</v>
-      </c>
-      <c r="B61" t="s">
-        <v>154</v>
-      </c>
-      <c r="C61" t="s">
-        <v>154</v>
-      </c>
-      <c r="E61" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
-      <c r="A63" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B63">
-        <v>101</v>
-      </c>
-      <c r="C63">
-        <v>101</v>
-      </c>
-      <c r="F63" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
-      <c r="A64" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B64">
-        <v>102</v>
-      </c>
-      <c r="C64">
-        <v>102</v>
-      </c>
-      <c r="F64" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
-      <c r="A65" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B65">
-        <v>103</v>
-      </c>
-      <c r="C65">
-        <v>103</v>
-      </c>
-      <c r="F65" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
-      <c r="A66" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B66">
-        <v>104</v>
-      </c>
-      <c r="C66">
-        <v>104</v>
-      </c>
-      <c r="F66" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
-      <c r="A67" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B67">
-        <v>105</v>
-      </c>
-      <c r="C67">
-        <v>105</v>
-      </c>
-      <c r="F67" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
-      <c r="A68" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B68">
-        <v>106</v>
-      </c>
-      <c r="C68">
-        <v>106</v>
-      </c>
-      <c r="F68" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6">
-      <c r="A69" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B69">
-        <v>107</v>
-      </c>
-      <c r="C69">
-        <v>107</v>
-      </c>
-      <c r="F69" t="s">
-        <v>137</v>
-      </c>
-    </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B70">
-        <v>108</v>
-      </c>
-      <c r="C70">
-        <v>108</v>
-      </c>
-      <c r="F70" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6">
-      <c r="A71" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B71">
-        <v>109</v>
-      </c>
-      <c r="C71">
-        <v>109</v>
-      </c>
-      <c r="F71" t="s">
-        <v>139</v>
+      <c r="A70" t="s">
+        <v>89</v>
+      </c>
+      <c r="B70" t="s">
+        <v>163</v>
+      </c>
+      <c r="C70" t="s">
+        <v>163</v>
+      </c>
+      <c r="E70" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2342,13 +2369,13 @@
         <v>111</v>
       </c>
       <c r="B72">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C72">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="F72" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2356,13 +2383,13 @@
         <v>111</v>
       </c>
       <c r="B73">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C73">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="F73" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -2370,13 +2397,13 @@
         <v>111</v>
       </c>
       <c r="B74">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C74">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="F74" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -2384,13 +2411,13 @@
         <v>111</v>
       </c>
       <c r="B75">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C75">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="F75" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -2398,13 +2425,13 @@
         <v>111</v>
       </c>
       <c r="B76">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="C76">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F76" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -2412,13 +2439,13 @@
         <v>111</v>
       </c>
       <c r="B77">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="C77">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F77" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -2426,13 +2453,13 @@
         <v>111</v>
       </c>
       <c r="B78">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C78">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="F78" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -2440,13 +2467,13 @@
         <v>111</v>
       </c>
       <c r="B79">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C79">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="F79" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -2454,13 +2481,13 @@
         <v>111</v>
       </c>
       <c r="B80">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C80">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="F80" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -2468,13 +2495,13 @@
         <v>111</v>
       </c>
       <c r="B81">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C81">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="F81" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -2482,13 +2509,13 @@
         <v>111</v>
       </c>
       <c r="B82">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C82">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="F82" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -2496,13 +2523,13 @@
         <v>111</v>
       </c>
       <c r="B83">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="C83">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="F83" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -2510,13 +2537,13 @@
         <v>111</v>
       </c>
       <c r="B84">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="C84">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="F84" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -2524,13 +2551,13 @@
         <v>111</v>
       </c>
       <c r="B85">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C85">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="F85" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -2538,19 +2565,257 @@
         <v>111</v>
       </c>
       <c r="B86">
+        <v>115</v>
+      </c>
+      <c r="C86">
+        <v>115</v>
+      </c>
+      <c r="F86" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B87">
+        <v>116</v>
+      </c>
+      <c r="C87">
+        <v>116</v>
+      </c>
+      <c r="F87" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B88">
+        <v>117</v>
+      </c>
+      <c r="C88">
+        <v>117</v>
+      </c>
+      <c r="F88" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B89">
+        <v>118</v>
+      </c>
+      <c r="C89">
+        <v>118</v>
+      </c>
+      <c r="F89" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B90">
+        <v>119</v>
+      </c>
+      <c r="C90">
+        <v>119</v>
+      </c>
+      <c r="F90" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B91">
+        <v>120</v>
+      </c>
+      <c r="C91">
+        <v>120</v>
+      </c>
+      <c r="F91" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B92">
+        <v>121</v>
+      </c>
+      <c r="C92">
+        <v>121</v>
+      </c>
+      <c r="F92" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B93">
+        <v>122</v>
+      </c>
+      <c r="C93">
+        <v>122</v>
+      </c>
+      <c r="F93" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B94">
+        <v>123</v>
+      </c>
+      <c r="C94">
+        <v>123</v>
+      </c>
+      <c r="F94" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B95">
         <v>124</v>
       </c>
-      <c r="C86">
+      <c r="C95">
         <v>124</v>
       </c>
-      <c r="F86" t="s">
+      <c r="F95" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B96">
+        <v>201</v>
+      </c>
+      <c r="C96">
+        <v>201</v>
+      </c>
+      <c r="F96" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B97">
+        <v>202</v>
+      </c>
+      <c r="C97">
+        <v>202</v>
+      </c>
+      <c r="F97" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B98">
+        <v>203</v>
+      </c>
+      <c r="C98">
+        <v>203</v>
+      </c>
+      <c r="F98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B99">
+        <v>204</v>
+      </c>
+      <c r="C99">
+        <v>204</v>
+      </c>
+      <c r="F99" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B100">
+        <v>205</v>
+      </c>
+      <c r="C100">
+        <v>205</v>
+      </c>
+      <c r="F100" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="A101" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B101">
+        <v>206</v>
+      </c>
+      <c r="C101">
+        <v>206</v>
+      </c>
+      <c r="F101" t="s">
         <v>154</v>
       </c>
     </row>
+    <row r="102" spans="1:6">
+      <c r="A102" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B102">
+        <v>207</v>
+      </c>
+      <c r="C102">
+        <v>207</v>
+      </c>
+      <c r="F102" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
+      <c r="A103" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B103">
+        <v>208</v>
+      </c>
+      <c r="C103">
+        <v>208</v>
+      </c>
+      <c r="F103" t="s">
+        <v>161</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A42:E49">
-    <sortCondition ref="A42:A49"/>
-    <sortCondition ref="E42:E49"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A43:E50">
+    <sortCondition ref="A43:A50"/>
+    <sortCondition ref="E43:E50"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2561,7 +2826,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2584,10 +2849,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="13" t="s">
-        <v>117</v>
+        <v>149</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>116</v>
+        <v>150</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>115</v>

</xml_diff>